<commit_message>
Work on CIN and ISA
</commit_message>
<xml_diff>
--- a/SPA/Proyectos/Husillo/Documentación/listaVariables.xlsx
+++ b/SPA/Proyectos/Husillo/Documentación/listaVariables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joel0\Documents\ARI\SPA\Proyectos\Husillo\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joel\Documents\ARI\SPA\Proyectos\Husillo\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623E1B65-7E9C-49F1-9524-FFF331711D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E40C53-E918-4837-9196-AFA90323557B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15885" xr2:uid="{B934DF4C-BF87-4FD7-A4DC-3729DB28A2DF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B934DF4C-BF87-4FD7-A4DC-3729DB28A2DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -160,39 +160,21 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -229,26 +211,58 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -269,7 +283,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -568,20 +582,20 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -598,98 +612,98 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="7" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>